<commit_message>
fix export booking file generation
</commit_message>
<xml_diff>
--- a/templates/jnt.xlsx
+++ b/templates/jnt.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sample-projects\edge-system\edge-node\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Ennovation\edge-system\edge-node\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -306,8 +306,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="184" formatCode="#,##0.00;[Red]#,##0.00"/>
-    <numFmt numFmtId="185" formatCode="#,##0;[Red]#,##0"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00;[Red]#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="#,##0;[Red]#,##0"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -504,7 +504,7 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="184" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -576,64 +576,64 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="184" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="184" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="184" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="184" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="184" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="184" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="184" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="184" fontId="18" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="184" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="37" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="185" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="184" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="37" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="185" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -990,7 +990,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M5098"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
@@ -1007,7 +1007,7 @@
     <col min="10" max="10" width="15.28515625" style="5" customWidth="1"/>
     <col min="11" max="11" width="14.5703125" style="4" customWidth="1"/>
     <col min="12" max="12" width="14.85546875" style="4" customWidth="1"/>
-    <col min="13" max="13" width="18.85546875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="52" style="2" customWidth="1"/>
     <col min="14" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>

</xml_diff>